<commit_message>
Setup done for Parallel Execution
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\Coding Round\TechMahindra_Code_Test\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627A9A10-4A7F-4AC7-BA6C-4527A149B765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{740F7B3C-9674-49BF-9E98-2481FDDD2DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,16 +30,16 @@
     <t>Input</t>
   </si>
   <si>
-    <t>5*3-4</t>
-  </si>
-  <si>
-    <t>90+200+1000-245</t>
-  </si>
-  <si>
     <t>7*4/2+6-3</t>
   </si>
   <si>
     <t>52+1+4+5-3*4</t>
+  </si>
+  <si>
+    <t>5*3-4+100</t>
+  </si>
+  <si>
+    <t>90+200+1000-245/10</t>
   </si>
 </sst>
 </file>
@@ -384,12 +384,12 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" style="4" customWidth="1"/>
     <col min="2" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -400,22 +400,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>